<commit_message>
- changes done after Sonarcube scan. - added new diagram - modified Lab01_ReviewReport.xlsx with all the changes required
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Laptop\e\VVSS\CamiVVSS_ro2024-2025\Labs\Lab01\CheckListsAll\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{89FD84A2-D8E1-420F-B67D-AE002DC5AD64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D7BBF9D-D3F8-4DC9-96B0-D27CF3ED4ACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="650" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="650" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="102">
   <si>
     <t>do not print this form</t>
   </si>
@@ -218,6 +218,9 @@
     <t>Controller ul foloseste metode pe tasklist direct, fara a apela la TaskService. De asemenea unele metode nu sunt folosite. eg. setTask din LinkedTaskList.java</t>
   </si>
   <si>
+    <t>x</t>
+  </si>
+  <si>
     <t>C06</t>
   </si>
   <si>
@@ -227,18 +230,27 @@
     <t>C11</t>
   </si>
   <si>
+    <t>TaskIO class</t>
+  </si>
+  <si>
+    <t>Exista variabile care nu sunt sugestive. "tks", "t", "fis", "p"</t>
+  </si>
+  <si>
+    <t>C04</t>
+  </si>
+  <si>
     <t>code-varriabile</t>
   </si>
   <si>
-    <t>Exista variabile care nu sunt sugestive. "tks", "t"</t>
-  </si>
-  <si>
-    <t>C04</t>
-  </si>
-  <si>
     <t>La apelarea showFilteredTasks, cand utilizatorul introduce un format gresit de date, avem eroare.</t>
   </si>
   <si>
+    <t>DateService, line 64</t>
+  </si>
+  <si>
+    <t>&gt; in loc de &gt;=. Se accepta si ora 24 sau minutul 60, ceea ce este gresit.</t>
+  </si>
+  <si>
     <t>2h</t>
   </si>
   <si>
@@ -258,6 +270,99 @@
   </si>
   <si>
     <t>After/Argument</t>
+  </si>
+  <si>
+    <t>29-TaskList.java</t>
+  </si>
+  <si>
+    <t>Standard outputs should not be used directly to log anything</t>
+  </si>
+  <si>
+    <t>System.out.println(getTask(i).getTitle());</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inter"/>
+      </rPr>
+      <t>log</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF000000"/>
+        <rFont val="Inter"/>
+      </rPr>
+      <t>.info(getTask(i).getTitle());</t>
+    </r>
+  </si>
+  <si>
+    <t>21- Main.java</t>
+  </si>
+  <si>
+    <t>Constant names should comply with a naming convention</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    private static final int defaultWidth = 820;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    private static final int DEFAULTWIDTTH= 820;
+</t>
+  </si>
+  <si>
+    <t>27 - Main.java</t>
+  </si>
+  <si>
+    <t>Unused "private" fields should be removed</t>
+  </si>
+  <si>
+    <t>private static ClassLoader classLoader = Main.class.getClassLoader();</t>
+  </si>
+  <si>
+    <t>We removed it :)</t>
+  </si>
+  <si>
+    <t>95-Task.java</t>
+  </si>
+  <si>
+    <t>Boolean checks should not be inverted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     return !(this.interval == 0);</t>
+  </si>
+  <si>
+    <t>return this.interval != 0;</t>
+  </si>
+  <si>
+    <t>30 - Main.java</t>
+  </si>
+  <si>
+    <t>Sections of code should not be commented out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    private TasksService service = new TasksService(savedTasksList);//savedTasksList);
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> we removed //savedTasksList);</t>
+  </si>
+  <si>
+    <t>57 - Main.java</t>
+  </si>
+  <si>
+    <t>Lambdas containing only one statement should not nest this statement in a block</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        primaryStage.setOnCloseRequest(we -&gt; {
+                System.exit(0);
+            });</t>
+  </si>
+  <si>
+    <t>Removing the curly braces is an useless procedure since future modifications to the code can use multiple arugments in that lambda function? (It doesn't look right without curly braces :D )</t>
   </si>
   <si>
     <t>Effort to perform tool-based code analysis (hours):</t>
@@ -267,7 +372,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -344,6 +449,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF000000"/>
+      <name val="Inter"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF000000"/>
+      <name val="Inter"/>
     </font>
   </fonts>
   <fills count="5">
@@ -445,7 +561,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -472,6 +588,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -516,8 +636,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -829,8 +951,8 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E13" sqref="B13:E13"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
@@ -855,20 +977,20 @@
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
       <c r="G1" s="16"/>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="16"/>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
       <c r="H2" s="18"/>
@@ -903,10 +1025,10 @@
       <c r="C4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="23"/>
+      <c r="E4" s="25"/>
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
       <c r="H4" s="18" t="s">
@@ -925,10 +1047,10 @@
       <c r="C5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="25"/>
+      <c r="E5" s="27"/>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
       <c r="H5" s="18" t="s">
@@ -947,8 +1069,8 @@
       <c r="C6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
       <c r="H6" s="16"/>
@@ -961,8 +1083,8 @@
       <c r="C7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
       <c r="H7" s="16"/>
@@ -1260,20 +1382,20 @@
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
       <c r="G1" s="16"/>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="16"/>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
       <c r="H2" s="18"/>
@@ -1308,10 +1430,10 @@
       <c r="C4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="26"/>
+      <c r="E4" s="28"/>
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
       <c r="H4" s="18" t="s">
@@ -1330,10 +1452,10 @@
       <c r="C5" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="28"/>
+      <c r="E5" s="30"/>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
       <c r="H5" s="18" t="s">
@@ -1352,8 +1474,8 @@
       <c r="C6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
       <c r="H6" s="16"/>
@@ -1366,8 +1488,8 @@
       <c r="C7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
       <c r="H7" s="16"/>
@@ -1420,13 +1542,13 @@
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="35" t="s">
+      <c r="D11" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="35" t="s">
+      <c r="E11" s="21" t="s">
         <v>47</v>
       </c>
       <c r="F11" s="16"/>
@@ -1441,13 +1563,13 @@
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="35" t="s">
+      <c r="E12" s="21" t="s">
         <v>48</v>
       </c>
       <c r="F12" s="16"/>
@@ -1649,8 +1771,8 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
@@ -1675,20 +1797,20 @@
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
       <c r="G1" s="16"/>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="16"/>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
       <c r="H2" s="18"/>
@@ -1723,10 +1845,10 @@
       <c r="C4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="E4" s="29"/>
+      <c r="E4" s="31"/>
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
       <c r="H4" s="18" t="s">
@@ -1745,10 +1867,10 @@
       <c r="C5" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="E5" s="31"/>
+      <c r="E5" s="33"/>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
       <c r="H5" s="18" t="s">
@@ -1767,8 +1889,8 @@
       <c r="C6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
       <c r="H6" s="16"/>
@@ -1781,8 +1903,8 @@
       <c r="C7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
       <c r="H7" s="16"/>
@@ -1823,7 +1945,9 @@
       <c r="E10" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F10" s="16"/>
+      <c r="F10" s="16" t="s">
+        <v>59</v>
+      </c>
       <c r="G10" s="16"/>
       <c r="H10" s="16"/>
       <c r="I10" s="16"/>
@@ -1836,15 +1960,17 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>49</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F11" s="16"/>
+        <v>61</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>59</v>
+      </c>
       <c r="G11" s="16"/>
       <c r="H11" s="16"/>
       <c r="I11" s="16"/>
@@ -1857,15 +1983,17 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F12" s="16"/>
+        <v>64</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>59</v>
+      </c>
       <c r="G12" s="16"/>
       <c r="H12" s="16"/>
       <c r="I12" s="16"/>
@@ -1878,30 +2006,40 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F13" s="16"/>
+        <v>67</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>59</v>
+      </c>
       <c r="G13" s="16"/>
       <c r="H13" s="16"/>
       <c r="I13" s="16"/>
       <c r="J13" s="16"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" ht="30.75">
       <c r="A14" s="16"/>
       <c r="B14" s="18">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="16"/>
+      <c r="C14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>59</v>
+      </c>
       <c r="G14" s="16"/>
       <c r="H14" s="16"/>
       <c r="I14" s="16"/>
@@ -2070,7 +2208,7 @@
       </c>
       <c r="D32" s="11"/>
       <c r="E32" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -2094,8 +2232,8 @@
   </sheetPr>
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
@@ -2121,20 +2259,20 @@
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
       <c r="G1" s="16"/>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="16"/>
-      <c r="B2" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
+      <c r="B2" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
       <c r="H2" s="18"/>
@@ -2167,10 +2305,10 @@
       <c r="A4" s="16"/>
       <c r="B4" s="16"/>
       <c r="C4" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
+        <v>72</v>
+      </c>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
       <c r="H4" s="18" t="s">
@@ -2189,8 +2327,8 @@
       <c r="C5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
       <c r="H5" s="18" t="s">
@@ -2209,8 +2347,8 @@
       <c r="C6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
       <c r="H6" s="16"/>
@@ -2223,112 +2361,160 @@
         <v>17</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="G9" s="16"/>
       <c r="H9" s="16"/>
       <c r="I9" s="16"/>
       <c r="J9" s="16"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" ht="60.75">
       <c r="A10" s="16"/>
       <c r="B10" s="18">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="C10" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E10" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="F10" s="37" t="s">
+        <v>80</v>
+      </c>
       <c r="G10" s="16"/>
       <c r="H10" s="16"/>
       <c r="I10" s="16"/>
       <c r="J10" s="16"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" ht="76.5">
       <c r="A11" s="16"/>
       <c r="B11" s="18">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="C11" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="G11" s="16"/>
       <c r="H11" s="16"/>
       <c r="I11" s="16"/>
       <c r="J11" s="16"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" ht="60.75">
       <c r="A12" s="16"/>
       <c r="B12" s="18">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="C12" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>88</v>
+      </c>
       <c r="G12" s="16"/>
       <c r="H12" s="16"/>
       <c r="I12" s="16"/>
       <c r="J12" s="16"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" ht="45.75">
       <c r="A13" s="16"/>
       <c r="B13" s="18">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="C13" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F13" s="36" t="s">
+        <v>92</v>
+      </c>
       <c r="G13" s="16"/>
       <c r="H13" s="16"/>
       <c r="I13" s="16"/>
       <c r="J13" s="16"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" ht="76.5">
       <c r="A14" s="16"/>
       <c r="B14" s="18">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="C14" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="G14" s="16"/>
       <c r="H14" s="16"/>
       <c r="I14" s="16"/>
       <c r="J14" s="16"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" ht="183">
       <c r="A15" s="16"/>
       <c r="B15" s="18">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+      <c r="C15" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>100</v>
+      </c>
       <c r="G15" s="16"/>
       <c r="H15" s="16"/>
       <c r="I15" s="16"/>
       <c r="J15" s="16"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" ht="15">
       <c r="A16" s="16"/>
       <c r="B16" s="18">
         <f t="shared" si="0"/>
@@ -2485,11 +2671,11 @@
     </row>
     <row r="32" spans="2:6">
       <c r="B32" s="16"/>
-      <c r="C32" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="D32" s="33"/>
-      <c r="E32" s="33"/>
+      <c r="C32" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="D32" s="35"/>
+      <c r="E32" s="35"/>
       <c r="F32" s="15"/>
     </row>
     <row r="35" spans="6:6">

</xml_diff>